<commit_message>
Updated test data for TC62
</commit_message>
<xml_diff>
--- a/Test Data/TC_62_Verify_Accessories_Gallery_Update_On_Max_Limit_Of_Slots_Available_For_Backplane_Are_Occupied.xlsx
+++ b/Test Data/TC_62_Verify_Accessories_Gallery_Update_On_Max_Limit_Of_Slots_Available_For_Backplane_Are_Occupied.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\consys-uiauto\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F575C77F-A94F-40E7-B8F8-9976BD9F9DD9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D89B3729-A2F6-4CC2-A9D3-489404E33CBC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="38">
   <si>
     <t>Color Codes</t>
   </si>
@@ -574,7 +574,7 @@
   <dimension ref="A1:P10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B4"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -827,11 +827,11 @@
       <c r="K10" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="L10" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="M10" s="14" t="s">
-        <v>21</v>
+      <c r="L10" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="M10" s="14" t="b">
+        <v>0</v>
       </c>
       <c r="N10" s="14" t="s">
         <v>34</v>

</xml_diff>

<commit_message>
Updated test data sheet for TC62
</commit_message>
<xml_diff>
--- a/Test Data/TC_62_Verify_Accessories_Gallery_Update_On_Max_Limit_Of_Slots_Available_For_Backplane_Are_Occupied.xlsx
+++ b/Test Data/TC_62_Verify_Accessories_Gallery_Update_On_Max_Limit_Of_Slots_Available_For_Backplane_Are_Occupied.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\consys-uiauto\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D89B3729-A2F6-4CC2-A9D3-489404E33CBC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17F7D358-703B-4A06-8EA6-C1EACE06E26A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Add Devices" sheetId="6" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="38">
   <si>
     <t>Color Codes</t>
   </si>
@@ -573,8 +573,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -856,8 +856,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F72A1DD-C6B1-422C-BE52-8341BCA3CA4F}">
   <dimension ref="A1:P10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1110,11 +1110,11 @@
       <c r="K10" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="L10" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="M10" s="14" t="s">
-        <v>21</v>
+      <c r="L10" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="M10" s="14" t="b">
+        <v>0</v>
       </c>
       <c r="N10" s="14" t="s">
         <v>34</v>

</xml_diff>